<commit_message>
New version of the data sheet
</commit_message>
<xml_diff>
--- a/Data of device.xlsx
+++ b/Data of device.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab programs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C149F113-E2CE-40D1-BF30-07526A2D5896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069AF095-CFCD-451D-AA7B-0F0A67457102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>Model</t>
   </si>
@@ -226,6 +226,122 @@
   </si>
   <si>
     <t>Load recommand: &gt;2k omes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DC 12 V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Larger Scale one'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6-12V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3W lens heat sink</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15 degrees for lens angle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>590-595nm(Yellow)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>440-445nm(Blue)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>520-525nm(Green)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>620-625nm(Red)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6000-6500K(White)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>piezoelectric</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12MM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20MM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brown 0.6mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>White 1mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Motor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>XD37GA-520YSY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DC 24V for maximum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>600 r/min for maximum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Seven modes for power supply:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12, 15, 16, 18, 19, 20, 24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T(emitter)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TCT40 - 16T/R-1.2.3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>140Vpp approximately for max</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>40KHz and 25KHz (Center)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ultrasound transducor</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -269,9 +385,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -610,19 +727,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="109" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
     <col min="2" max="2" width="20.6640625" customWidth="1"/>
     <col min="3" max="3" width="23.83203125" customWidth="1"/>
     <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="5" width="20.75" customWidth="1"/>
+    <col min="5" max="5" width="28.08203125" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" customWidth="1"/>
     <col min="7" max="7" width="38.1640625" customWidth="1"/>
   </cols>
@@ -806,6 +923,127 @@
         <v>45</v>
       </c>
     </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" t="s">
+        <v>69</v>
+      </c>
+      <c r="G35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G37" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New version data and create the feature for Arduino.
</commit_message>
<xml_diff>
--- a/Data of device.xlsx
+++ b/Data of device.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab programs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069AF095-CFCD-451D-AA7B-0F0A67457102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E0CC80-7C65-4128-A88F-789A1692CBFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>Model</t>
   </si>
@@ -342,6 +342,30 @@
   </si>
   <si>
     <t>Ultrasound transducor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mirror</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Focal Length: 1.6m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Arduino</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZYDUINO UNO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5V for operating voltage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7-12V for input voltage</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -404,10 +428,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -727,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="109" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="113" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1044,6 +1064,30 @@
         <v>76</v>
       </c>
     </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>78</v>
+      </c>
+      <c r="G43" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>80</v>
+      </c>
+      <c r="B45" t="s">
+        <v>81</v>
+      </c>
+      <c r="C45" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C46" t="s">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New version of Data sheet.
</commit_message>
<xml_diff>
--- a/Data of device.xlsx
+++ b/Data of device.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab programs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B26F223D-45E6-4C28-A1D6-FC29A62EE884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8262C423-FC76-4FEA-8EFC-88D4B84CD5A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="104">
   <si>
     <t>Model</t>
   </si>
@@ -406,6 +406,46 @@
   </si>
   <si>
     <t>S for GND and D for output voltage pin.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sine wave mode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Frequency</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 - 65.789Hz; 526.32 Hz; 7KHz; 94.34KHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Triangular wave mode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Peak to Peak</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>18V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Square</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13.5V</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -449,10 +489,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -787,10 +830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E41" zoomScale="113" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+    <sheetView tabSelected="1" topLeftCell="F6" zoomScale="113" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -802,9 +845,12 @@
     <col min="5" max="5" width="28.08203125" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" customWidth="1"/>
     <col min="7" max="7" width="38.1640625" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" customWidth="1"/>
+    <col min="9" max="9" width="32.4140625" customWidth="1"/>
+    <col min="10" max="10" width="18.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -821,7 +867,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -838,7 +884,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -858,10 +904,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -881,17 +927,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -911,258 +957,295 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="I10" t="s">
+        <v>94</v>
+      </c>
+      <c r="J10" t="s">
+        <v>97</v>
+      </c>
+      <c r="K10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H11" t="s">
+        <v>95</v>
+      </c>
+      <c r="I11" t="s">
+        <v>96</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H12" t="s">
+        <v>99</v>
+      </c>
+      <c r="I12" t="s">
+        <v>102</v>
+      </c>
+      <c r="J12" t="s">
+        <v>100</v>
+      </c>
+      <c r="K12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>29</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B15" t="s">
         <v>30</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C15" t="s">
         <v>43</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D15" t="s">
         <v>32</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D13" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>35</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B18" t="s">
         <v>36</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C18" t="s">
         <v>37</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D18" t="s">
         <v>38</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E18" t="s">
         <v>39</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G18" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17" t="s">
-        <v>47</v>
-      </c>
-      <c r="G17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C18" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>49</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C23" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C25" t="s">
         <v>53</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E25" t="s">
         <v>54</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G25" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G23" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G25" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G26" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G30" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B32" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>67</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B38" t="s">
         <v>68</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C38" t="s">
         <v>69</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G38" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G36" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G39" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G37" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G40" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>77</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B42" t="s">
         <v>73</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C42" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B40" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>78</v>
       </c>
-      <c r="G43" t="s">
+      <c r="G46" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>80</v>
-      </c>
-      <c r="B45" t="s">
-        <v>81</v>
-      </c>
-      <c r="C45" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C46" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>80</v>
+      </c>
+      <c r="B48" t="s">
+        <v>81</v>
+      </c>
+      <c r="C48" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>84</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B51" t="s">
         <v>85</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C51" t="s">
         <v>88</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D51" t="s">
         <v>90</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G51" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C49" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
         <v>89</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D52" t="s">
         <v>91</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G52" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="G50" t="s">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G53" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="G51" t="s">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G54" t="s">
         <v>93</v>
       </c>
     </row>

</xml_diff>